<commit_message>
Added 1% resistors to Master Parts List
</commit_message>
<xml_diff>
--- a/Master_Parts_List_Newark.xlsx
+++ b/Master_Parts_List_Newark.xlsx
@@ -94,9 +94,11 @@
           </table:table-cell>
           <table:covered-table-cell table:number-columns-repeated="74"/>
         </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string" table:number-columns-spanned="75" table:number-rows-spanned="1">
-            <text:p>RESISTORS</text:p>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string" table:number-columns-spanned="75" table:number-rows-spanned="1">
+            <text:p>
+              <text:a xlink:href="https://www.newark.com/vishay/mba02040c2052frp00/resistor-metal-film-20-5kohm-400mw/dp/94C3403" xlink:type="simple">https://www.newark.com/vishay/mba02040c2052frp00/resistor-metal-film-20-5kohm-400mw/dp/94C3403</text:a>
+            </text:p>
           </table:table-cell>
           <table:covered-table-cell table:number-columns-repeated="74"/>
         </table:table-row>
@@ -239,11 +241,11 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2025-02-02T20:47:14.198071765</meta:creation-date>
-    <dc:date>2025-02-02T20:50:01.737587179</dc:date>
-    <meta:editing-duration>PT2M49S</meta:editing-duration>
-    <meta:editing-cycles>1</meta:editing-cycles>
+    <dc:date>2025-02-02T21:01:21.496496769</dc:date>
+    <meta:editing-duration>PT3M</meta:editing-duration>
+    <meta:editing-cycles>2</meta:editing-cycles>
+    <meta:generator>LibreOffice/24.8.3.2$Linux_X86_64 LibreOffice_project/e14c9fdd1f585efcbb2c5363087a99d20928d522</meta:generator>
     <meta:document-statistic meta:table-count="1" meta:cell-count="8" meta:object-count="0"/>
-    <meta:generator>LibreOffice/24.8.3.2$Linux_X86_64 LibreOffice_project/e14c9fdd1f585efcbb2c5363087a99d20928d522</meta:generator>
   </office:meta>
 </office:document-meta>
 </file>
@@ -255,14 +257,14 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">2258</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">3581</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">3575</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
               <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">8</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">21</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
@@ -279,7 +281,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Sheet1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">860</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">861</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -330,9 +332,9 @@
       <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
       <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string"/>
+      <config:config-item config:name="PrinterName" config:type="string">HP_OfficeJet_Pro_9010_series_CF5C38</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary"/>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">8AH+/0hQX09mZmljZUpldF9Qcm9fOTAxMF9zZXJpZXNfQ0Y1QzM4AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAQ1VQUzpIUF9PZmZpY2VKZXRfUHJvXzkwMTBfc2VyaQAWAAMApwAAAAAAAAAIAFZUAAAkbQAASm9iRGF0YSAxCnByaW50ZXI9SFBfT2ZmaWNlSmV0X1Byb185MDEwX3Nlcmllc19DRjVDMzgKb3JpZW50YXRpb249UG9ydHJhaXQKY29waWVzPTEKY29sbGF0ZT1mYWxzZQptYXJnaW5hZGp1c3RtZW50PTAsMCwnMCwwCmNvbG9yZGVwdGg9MjQKY29sb3JkZXZpY2U9MApQUERDb250ZXh0RGF0YQoSAENPTVBBVF9EVVBMRVhfTU9ERQ8ARHVwbGV4TW9kZTo6T2ZmDABQUklOVEVSX05BTUUjAEhQX09mZmljZUpldF9Qcm9fOTAxMF9zZXJpZXNfQ0Y1QzM4CwBEUklWRVJfTkFNRSgAQ1VQUzpIUF9PZmZpY2VKZXRfUHJvXzkwMTBfc2VyaWVzX0NGNUMzOA==</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
@@ -346,6 +348,7 @@
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
       <config:config-item-map-named config:name="ScriptConfiguration">
         <config:config-item-map-entry config:name="Sheet1">
@@ -371,7 +374,7 @@
     </style:default-style>
     <style:default-style style:family="graphic">
       <style:graphic-properties svg:stroke-color="#3465a4" draw:fill-color="#729fcf" fo:wrap-option="no-wrap" draw:shadow-offset-x="0.1181in" draw:shadow-offset-y="0.1181in" style:writing-mode="page"/>
-      <style:paragraph-properties style:text-autospace="ideograph-alpha" style:punctuation-wrap="simple" style:line-break="strict" style:writing-mode="page" style:font-independent-line-spacing="false">
+      <style:paragraph-properties style:text-autospace="ideograph-alpha" style:punctuation-wrap="simple" style:line-break="strict" loext:tab-stop-distance="0in" style:writing-mode="page" style:font-independent-line-spacing="false">
         <style:tab-stops/>
       </style:paragraph-properties>
       <style:text-properties style:use-window-font-color="true" loext:opacity="0%" fo:font-family="'Liberation Serif'" style:font-family-generic="roman" style:font-pitch="variable" fo:font-size="12pt" fo:language="en" fo:country="US" style:letter-kerning="true" style:font-family-asian="'DejaVu Sans'" style:font-family-generic-asian="system" style:font-pitch-asian="variable" style:font-size-asian="12pt" style:language-asian="zh" style:country-asian="CN" style:font-family-complex="'Noto Sans'" style:font-family-generic-complex="system" style:font-pitch-complex="variable" style:font-size-complex="12pt" style:language-complex="hi" style:country-complex="IN"/>
@@ -532,7 +535,7 @@
           <text:p>
             <text:date style:data-style-name="N2" text:date-value="2025-02-02">00/00/0000</text:date>
             , 
-            <text:time>00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="21:01:09.745381159">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>